<commit_message>
August 7th second commit
</commit_message>
<xml_diff>
--- a/xydata.xlsx
+++ b/xydata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\jakkalavanya1 GITHUB\MATLAB_MDV-CAVsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1C0BA7B-DF67-4F96-9A76-13A6CA1088DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1DB1FE25-0C44-42B6-926D-D13D37E5668A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9.5312169113715868</v>
+        <v>9.3115439969289042</v>
       </c>
       <c r="B21">
-        <v>9.3819506023751984</v>
+        <v>9.2334896323687872</v>
       </c>
       <c r="C21">
         <v>-14.887999999999973</v>
@@ -1038,7 +1038,7 @@
         <v>107.625</v>
       </c>
       <c r="F21">
-        <v>2.3454876505937996</v>
+        <v>2.3083724080921968</v>
       </c>
       <c r="G21">
         <v>107.625</v>
@@ -1055,28 +1055,28 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>17.461225294095243</v>
+        <v>16.602819080228556</v>
       </c>
       <c r="B22">
-        <v>16.878509724276924</v>
+        <v>16.296444841648466</v>
       </c>
       <c r="C22">
-        <v>-8.6472219660359517</v>
+        <v>-8.9411991569598328</v>
       </c>
       <c r="D22">
-        <v>-48.647221966035922</v>
+        <v>-48.941199156959797</v>
       </c>
       <c r="E22">
         <v>107.625</v>
       </c>
       <c r="F22">
-        <v>4.219627431069231</v>
+        <v>4.0741112104121164</v>
       </c>
       <c r="G22">
         <v>107.625</v>
       </c>
       <c r="H22">
-        <v>-12.16180549150898</v>
+        <v>-12.235299789239949</v>
       </c>
       <c r="I22">
         <v>107.625</v>
@@ -1087,28 +1087,28 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>26.146561616314472</v>
+        <v>24.26078988765147</v>
       </c>
       <c r="B23">
-        <v>24.867738336906626</v>
+        <v>23.584595093606353</v>
       </c>
       <c r="C23">
-        <v>-1.8996049269884523</v>
+        <v>-2.7638680037943057</v>
       </c>
       <c r="D23">
-        <v>-42.899604926988424</v>
+        <v>-43.763868003794272</v>
       </c>
       <c r="E23">
         <v>107.625</v>
       </c>
       <c r="F23">
-        <v>6.2169345842266566</v>
+        <v>5.8961487734015883</v>
       </c>
       <c r="G23">
         <v>107.625</v>
       </c>
       <c r="H23">
-        <v>-10.724901231747106</v>
+        <v>-10.940967000948568</v>
       </c>
       <c r="I23">
         <v>107.625</v>
@@ -1119,28 +1119,28 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>35.537362352049911</v>
+        <v>32.266021055658157</v>
       </c>
       <c r="B24">
-        <v>33.321297411132349</v>
+        <v>31.087269856819191</v>
       </c>
       <c r="C24">
-        <v>5.3265120882686467</v>
+        <v>3.6333229265156506</v>
       </c>
       <c r="D24">
-        <v>-36.673487911731328</v>
+        <v>-38.366677073484318</v>
       </c>
       <c r="E24">
         <v>107.625</v>
       </c>
       <c r="F24">
-        <v>8.3303243527830872</v>
+        <v>7.7718174642047977</v>
       </c>
       <c r="G24">
         <v>107.625</v>
       </c>
       <c r="H24">
-        <v>-9.1683719779328321</v>
+        <v>-9.5916692683710796</v>
       </c>
       <c r="I24">
         <v>107.625</v>
@@ -1151,28 +1151,28 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>45.5837639714332</v>
+        <v>40.599077223117263</v>
       </c>
       <c r="B25">
-        <v>42.210847919675473</v>
+        <v>38.793798598226871</v>
       </c>
       <c r="C25">
-        <v>12.179318340018602</v>
+        <v>10.856779271924728</v>
       </c>
       <c r="D25">
-        <v>-29.997209949159124</v>
+        <v>-32.76029689895298</v>
       </c>
       <c r="E25">
         <v>107.625</v>
       </c>
       <c r="F25">
-        <v>10.552711979918868</v>
+        <v>9.6984496495567178</v>
       </c>
       <c r="G25">
         <v>107.625</v>
       </c>
       <c r="H25">
-        <v>-7.4993024872897811</v>
+        <v>-8.190074224738245</v>
       </c>
       <c r="I25">
         <v>107.625</v>
@@ -1183,28 +1183,28 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>56.235902947543821</v>
+        <v>49.240523025829305</v>
       </c>
       <c r="B26">
-        <v>51.508050831062945</v>
+        <v>46.693510783463807</v>
       </c>
       <c r="C26">
-        <v>19.019624591768554</v>
+        <v>18.067735617333803</v>
       </c>
       <c r="D26">
-        <v>-22.899110068053446</v>
+        <v>-26.955398013114841</v>
       </c>
       <c r="E26">
         <v>107.625</v>
       </c>
       <c r="F26">
-        <v>12.877012707765736</v>
+        <v>11.673377695865952</v>
       </c>
       <c r="G26">
         <v>107.625</v>
       </c>
       <c r="H26">
-        <v>-5.7247775170133615</v>
+        <v>-6.7388495032787104</v>
       </c>
       <c r="I26">
         <v>107.625</v>
@@ -1215,28 +1215,28 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>67.443915750300619</v>
+        <v>58.170923103387764</v>
       </c>
       <c r="B27">
-        <v>61.184567115474465</v>
+        <v>54.775735882516742</v>
       </c>
       <c r="C27">
-        <v>25.847430843518509</v>
+        <v>25.266191962742877</v>
       </c>
       <c r="D27">
-        <v>-15.407527297324727</v>
+        <v>-20.962650948926324</v>
       </c>
       <c r="E27">
         <v>107.625</v>
       </c>
       <c r="F27">
-        <v>15.296141778868616</v>
+        <v>13.693933970629185</v>
       </c>
       <c r="G27">
         <v>107.625</v>
       </c>
       <c r="H27">
-        <v>-3.8518818243311816</v>
+        <v>-5.240662737231581</v>
       </c>
       <c r="I27">
         <v>107.625</v>
@@ -1247,28 +1247,28 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>79.157938852345637</v>
+        <v>67.370842087506418</v>
       </c>
       <c r="B28">
-        <v>71.212057747985341</v>
+        <v>63.02980335860866</v>
       </c>
       <c r="C28">
-        <v>32.662737095268461</v>
+        <v>32.452148308151955</v>
       </c>
       <c r="D28">
-        <v>-7.5508006659562739</v>
+        <v>-14.792726239306925</v>
       </c>
       <c r="E28">
         <v>107.625</v>
       </c>
       <c r="F28">
-        <v>17.803014436996335</v>
+        <v>15.757450839652165</v>
       </c>
       <c r="G28">
         <v>107.625</v>
       </c>
       <c r="H28">
-        <v>-1.8877001664890685</v>
+        <v>-3.6981815598267311</v>
       </c>
       <c r="I28">
         <v>107.625</v>
@@ -1279,28 +1279,28 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>91.328108727287599</v>
+        <v>76.820844619583283</v>
       </c>
       <c r="B29">
-        <v>81.562183698067088</v>
+        <v>71.445042683074576</v>
       </c>
       <c r="C29">
-        <v>39.465543347018418</v>
+        <v>39.625604653561034</v>
       </c>
       <c r="D29">
-        <v>0.64273079738357453</v>
+        <v>-8.4562944172661876</v>
       </c>
       <c r="E29">
         <v>107.625</v>
       </c>
       <c r="F29">
-        <v>20.390545924516772</v>
+        <v>17.861260670768644</v>
       </c>
       <c r="G29">
         <v>107.625</v>
       </c>
       <c r="H29">
-        <v>0.16068269934589363</v>
+        <v>-2.1140736043165469</v>
       </c>
       <c r="I29">
         <v>107.625</v>
@@ -1311,28 +1311,28 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>103.90456184366383</v>
+        <v>86.50149533653655</v>
       </c>
       <c r="B30">
-        <v>92.206605940080692</v>
+        <v>80.01078331730281</v>
       </c>
       <c r="C30">
-        <v>46.255849598768371</v>
+        <v>46.78656099897011</v>
       </c>
       <c r="D30">
-        <v>8.228878572696452</v>
+        <v>-1.9640260156100577</v>
       </c>
       <c r="E30">
         <v>107.625</v>
       </c>
       <c r="F30">
-        <v>23.051651485020173</v>
+        <v>20.002695829325702</v>
       </c>
       <c r="G30">
         <v>107.625</v>
       </c>
       <c r="H30">
-        <v>2.057219643174113</v>
+        <v>-0.49100650390251444</v>
       </c>
       <c r="I30">
         <v>107.625</v>
@@ -1343,28 +1343,28 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>116.83743467840452</v>
+        <v>96.393358873370346</v>
       </c>
       <c r="B31">
-        <v>103.11698544461967</v>
+        <v>88.716354733805758</v>
       </c>
       <c r="C31">
-        <v>53.033655850518322</v>
+        <v>53.935017344379183</v>
       </c>
       <c r="D31">
-        <v>15.802526348009328</v>
+        <v>4.6734084326446776</v>
       </c>
       <c r="E31">
         <v>107.625</v>
       </c>
       <c r="F31">
-        <v>25.779246361154918</v>
+        <v>22.17908868345144</v>
       </c>
       <c r="G31">
         <v>107.625</v>
       </c>
       <c r="H31">
-        <v>3.9506315870023321</v>
+        <v>1.1683521081611694</v>
       </c>
       <c r="I31">
         <v>107.625</v>
@@ -1375,28 +1375,28 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>130.07686369288911</v>
+        <v>106.47699987570905</v>
       </c>
       <c r="B32">
-        <v>114.26498317665778</v>
+        <v>97.551086394356076</v>
       </c>
       <c r="C32">
-        <v>59.798962102268277</v>
+        <v>61.070973689788261</v>
       </c>
       <c r="D32">
-        <v>23.363674123322205</v>
+        <v>11.569770065103539</v>
       </c>
       <c r="E32">
         <v>107.625</v>
       </c>
       <c r="F32">
-        <v>28.566245794164445</v>
+        <v>24.387771598589019</v>
       </c>
       <c r="G32">
         <v>107.625</v>
       </c>
       <c r="H32">
-        <v>5.8409185308305513</v>
+        <v>2.8924425162758847</v>
       </c>
       <c r="I32">
         <v>107.625</v>
@@ -1407,28 +1407,28 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>143.57298535773384</v>
+        <v>116.73298297308554</v>
       </c>
       <c r="B33">
-        <v>125.62226012603736</v>
+        <v>106.50430777430998</v>
       </c>
       <c r="C33">
-        <v>66.551768354018236</v>
+        <v>68.194430035197342</v>
       </c>
       <c r="D33">
-        <v>30.912321898635081</v>
+        <v>18.4536316975624</v>
       </c>
       <c r="E33">
         <v>107.625</v>
       </c>
       <c r="F33">
-        <v>31.40556503150934</v>
+        <v>26.626076943577495</v>
       </c>
       <c r="G33">
         <v>107.625</v>
       </c>
       <c r="H33">
-        <v>7.7280804746587703</v>
+        <v>4.6134079243906001</v>
       </c>
       <c r="I33">
         <v>107.625</v>
@@ -1439,28 +1439,28 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>157.27593614959687</v>
+        <v>127.14187281044033</v>
       </c>
       <c r="B34">
-        <v>137.16047724008649</v>
+        <v>115.56534833561335</v>
       </c>
       <c r="C34">
-        <v>73.292074605768192</v>
+        <v>75.305386380606421</v>
       </c>
       <c r="D34">
-        <v>38.448469673947955</v>
+        <v>25.324993330021261</v>
       </c>
       <c r="E34">
         <v>107.625</v>
       </c>
       <c r="F34">
-        <v>34.290119310021623</v>
+        <v>28.891337083903338</v>
       </c>
       <c r="G34">
         <v>107.625</v>
       </c>
       <c r="H34">
-        <v>9.6121174184869886</v>
+        <v>6.3312483325053153</v>
       </c>
       <c r="I34">
         <v>107.625</v>
@@ -1471,28 +1471,28 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>171.13585251784764</v>
+        <v>137.68423401679848</v>
       </c>
       <c r="B35">
-        <v>148.85129548309192</v>
+        <v>124.72353753834071</v>
       </c>
       <c r="C35">
-        <v>80.01988085751816</v>
+        <v>82.403842726015498</v>
       </c>
       <c r="D35">
-        <v>45.972117449260828</v>
+        <v>32.183854962480119</v>
       </c>
       <c r="E35">
         <v>107.625</v>
       </c>
       <c r="F35">
-        <v>37.212823870772979</v>
+        <v>31.180884384585177</v>
       </c>
       <c r="G35">
         <v>107.625</v>
       </c>
       <c r="H35">
-        <v>11.493029362315207</v>
+        <v>8.0459637406200297</v>
       </c>
       <c r="I35">
         <v>107.625</v>
@@ -1503,28 +1503,28 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>185.10287097855996</v>
+        <v>148.34063122157733</v>
       </c>
       <c r="B36">
-        <v>160.6663758462675</v>
+        <v>133.96820485777997</v>
       </c>
       <c r="C36">
-        <v>86.735187109268125</v>
+        <v>89.489799071424585</v>
       </c>
       <c r="D36">
-        <v>53.483265224573707</v>
+        <v>39.030216594938977</v>
       </c>
       <c r="E36">
         <v>107.625</v>
       </c>
       <c r="F36">
-        <v>40.166593961566875</v>
+        <v>33.492051214444992</v>
       </c>
       <c r="G36">
         <v>107.625</v>
       </c>
       <c r="H36">
-        <v>13.370816306143427</v>
+        <v>9.7575541487347444</v>
       </c>
       <c r="I36">
         <v>107.625</v>
@@ -1535,28 +1535,28 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>199.12712796263793</v>
+        <v>159.09162907817421</v>
       </c>
       <c r="B37">
-        <v>172.57737931139343</v>
+        <v>143.2886797574325</v>
       </c>
       <c r="C37">
-        <v>93.437993361018087</v>
+        <v>96.56325541683367</v>
       </c>
       <c r="D37">
-        <v>60.981912999886582</v>
+        <v>45.864078227397833</v>
       </c>
       <c r="E37">
         <v>107.625</v>
       </c>
       <c r="F37">
-        <v>43.144344827848357</v>
+        <v>35.822169939358126</v>
       </c>
       <c r="G37">
         <v>107.625</v>
       </c>
       <c r="H37">
-        <v>15.245478249971645</v>
+        <v>11.466019556849458</v>
       </c>
       <c r="I37">
         <v>107.625</v>
@@ -1567,28 +1567,28 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>213.15875992940084</v>
+        <v>169.91779219010539</v>
       </c>
       <c r="B38">
-        <v>184.55596680321253</v>
+        <v>152.67429171448256</v>
       </c>
       <c r="C38">
-        <v>100.12829961276805</v>
+        <v>103.62421176224275</v>
       </c>
       <c r="D38">
-        <v>68.468060775199461</v>
+        <v>52.685439859856693</v>
       </c>
       <c r="E38">
         <v>107.625</v>
       </c>
       <c r="F38">
-        <v>46.138991700803132</v>
+        <v>38.168572928620641</v>
       </c>
       <c r="G38">
         <v>107.625</v>
       </c>
       <c r="H38">
-        <v>17.117015193799865</v>
+        <v>13.171359964964173</v>
       </c>
       <c r="I38">
         <v>107.625</v>
@@ -1599,28 +1599,28 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>227.14790349142868</v>
+        <v>180.79968523413226</v>
       </c>
       <c r="B39">
-        <v>196.57379935956988</v>
+        <v>162.11437021090521</v>
       </c>
       <c r="C39">
-        <v>106.806105864518</v>
+        <v>110.67266810765183</v>
       </c>
       <c r="D39">
-        <v>75.941708550512345</v>
+        <v>59.49430149231555</v>
       </c>
       <c r="E39">
         <v>107.625</v>
       </c>
       <c r="F39">
-        <v>49.143449839892469</v>
+        <v>40.528592552726302</v>
       </c>
       <c r="G39">
         <v>107.625</v>
       </c>
       <c r="H39">
-        <v>18.985427137628086</v>
+        <v>14.873575373078888</v>
       </c>
       <c r="I39">
         <v>107.625</v>
@@ -1631,28 +1631,28 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>241.04469499507479</v>
+        <v>191.71787285227276</v>
       </c>
       <c r="B40">
-        <v>208.60253793362028</v>
+        <v>171.59824464846395</v>
       </c>
       <c r="C40">
-        <v>113.47141211626797</v>
+        <v>117.70862445306091</v>
       </c>
       <c r="D40">
-        <v>83.402856325825226</v>
+        <v>66.290663124774412</v>
       </c>
       <c r="E40">
         <v>107.625</v>
       </c>
       <c r="F40">
-        <v>52.150634483405071</v>
+        <v>42.899561162115987</v>
       </c>
       <c r="G40">
         <v>107.625</v>
       </c>
       <c r="H40">
-        <v>20.850714081456307</v>
+        <v>16.572665781193603</v>
       </c>
       <c r="I40">
         <v>107.625</v>
@@ -1663,28 +1663,28 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>254.79927083366624</v>
+        <v>202.65291964292129</v>
       </c>
       <c r="B41">
-        <v>220.61384340383739</v>
+        <v>181.11524453523515</v>
       </c>
       <c r="C41">
-        <v>120.12421836801794</v>
+        <v>124.73208079846999</v>
       </c>
       <c r="D41">
-        <v>90.851504101138104</v>
+        <v>73.074524757233277</v>
       </c>
       <c r="E41">
         <v>107.625</v>
       </c>
       <c r="F41">
-        <v>55.153460850959348</v>
+        <v>45.278811133808787</v>
       </c>
       <c r="G41">
         <v>107.625</v>
       </c>
       <c r="H41">
-        <v>22.712876025284526</v>
+        <v>18.268631189308319</v>
       </c>
       <c r="I41">
         <v>107.625</v>
@@ -1695,28 +1695,28 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>268.3617675295958</v>
+        <v>213.58539027520439</v>
       </c>
       <c r="B42">
-        <v>232.57937696909073</v>
+        <v>190.65469934511577</v>
       </c>
       <c r="C42">
-        <v>126.7645246197679</v>
+        <v>131.74303714387906</v>
       </c>
       <c r="D42">
-        <v>98.28765187645098</v>
+        <v>79.84588638969214</v>
       </c>
       <c r="E42">
         <v>107.625</v>
       </c>
       <c r="F42">
-        <v>58.144844242272683</v>
+        <v>47.663674836278943</v>
       </c>
       <c r="G42">
         <v>107.625</v>
       </c>
       <c r="H42">
-        <v>24.571912969112745</v>
+        <v>19.961471597423035</v>
       </c>
       <c r="I42">
         <v>107.625</v>
@@ -1727,28 +1727,28 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>281.68232159918193</v>
+        <v>224.49584939101339</v>
       </c>
       <c r="B43">
-        <v>244.4707993487998</v>
+        <v>200.205938566746</v>
       </c>
       <c r="C43">
-        <v>133.39233087151786</v>
+        <v>138.74149348928816</v>
       </c>
       <c r="D43">
-        <v>105.71129965176387</v>
+        <v>86.604748022151</v>
       </c>
       <c r="E43">
         <v>107.625</v>
       </c>
       <c r="F43">
-        <v>61.11769983719995</v>
+        <v>50.0514846416865</v>
       </c>
       <c r="G43">
         <v>107.625</v>
       </c>
       <c r="H43">
-        <v>26.427824912940967</v>
+        <v>21.65118700553775</v>
       </c>
       <c r="I43">
         <v>107.625</v>
@@ -1759,28 +1759,28 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>294.71107033599878</v>
+        <v>235.36486152328376</v>
       </c>
       <c r="B44">
-        <v>256.25977141886176</v>
+        <v>209.75829160346126</v>
       </c>
       <c r="C44">
-        <v>140.00763712326781</v>
+        <v>145.72744983469724</v>
       </c>
       <c r="D44">
-        <v>113.12244742707675</v>
+        <v>93.351109654609871</v>
       </c>
       <c r="E44">
         <v>107.625</v>
       </c>
       <c r="F44">
-        <v>64.06494285471544</v>
+        <v>52.439572900865315</v>
       </c>
       <c r="G44">
         <v>107.625</v>
       </c>
       <c r="H44">
-        <v>28.280611856769188</v>
+        <v>23.337777413652468</v>
       </c>
       <c r="I44">
         <v>107.625</v>
@@ -1791,28 +1791,28 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>307.39815070068062</v>
+        <v>246.17299144780156</v>
       </c>
       <c r="B45">
-        <v>267.91795444023677</v>
+        <v>219.30108800320585</v>
       </c>
       <c r="C45">
-        <v>146.61044337501778</v>
+        <v>152.70090618010633</v>
       </c>
       <c r="D45">
-        <v>120.52109520238963</v>
+        <v>100.08497128706874</v>
       </c>
       <c r="E45">
         <v>107.625</v>
       </c>
       <c r="F45">
-        <v>66.979488610059192</v>
+        <v>54.825272000801462</v>
       </c>
       <c r="G45">
         <v>107.625</v>
       </c>
       <c r="H45">
-        <v>30.130273800597408</v>
+        <v>25.021242821767185</v>
       </c>
       <c r="I45">
         <v>107.625</v>
@@ -1823,28 +1823,28 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>319.6936959926411</v>
+        <v>256.90080378502182</v>
       </c>
       <c r="B46">
-        <v>279.41700923584369</v>
+        <v>228.82365722061047</v>
       </c>
       <c r="C46">
-        <v>153.20074962676773</v>
+        <v>159.6618625255154</v>
       </c>
       <c r="D46">
-        <v>127.90724297770251</v>
+        <v>106.80633291952761</v>
       </c>
       <c r="E46">
         <v>107.625</v>
       </c>
       <c r="F46">
-        <v>69.854252308960923</v>
+        <v>57.205914305152618</v>
       </c>
       <c r="G46">
         <v>107.625</v>
       </c>
       <c r="H46">
-        <v>31.976810744425627</v>
+        <v>26.701583229881901</v>
       </c>
       <c r="I46">
         <v>107.625</v>
@@ -1855,28 +1855,28 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>331.54784088877398</v>
+        <v>267.52886337581299</v>
       </c>
       <c r="B47">
-        <v>290.72859729702145</v>
+        <v>238.315328769345</v>
       </c>
       <c r="C47">
-        <v>159.77855587851769</v>
+        <v>166.61031887092449</v>
       </c>
       <c r="D47">
-        <v>135.2808907530154</v>
+        <v>113.51519455198647</v>
       </c>
       <c r="E47">
         <v>107.625</v>
       </c>
       <c r="F47">
-        <v>72.682149324255363</v>
+        <v>59.57883219233625</v>
       </c>
       <c r="G47">
         <v>107.625</v>
       </c>
       <c r="H47">
-        <v>33.82022268825385</v>
+        <v>28.378798637996617</v>
       </c>
       <c r="I47">
         <v>107.625</v>
@@ -1887,28 +1887,28 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>342.91073799225114</v>
+        <v>278.03773509143434</v>
       </c>
       <c r="B48">
-        <v>301.82437950158931</v>
+        <v>247.7654319169942</v>
       </c>
       <c r="C48">
-        <v>166.34386213026767</v>
+        <v>173.54627521633356</v>
       </c>
       <c r="D48">
-        <v>142.64203852832827</v>
+        <v>120.21155618444533</v>
       </c>
       <c r="E48">
         <v>107.625</v>
       </c>
       <c r="F48">
-        <v>75.456094875397326</v>
+        <v>61.941357979248551</v>
       </c>
       <c r="G48">
         <v>107.625</v>
       </c>
       <c r="H48">
-        <v>35.660509632082068</v>
+        <v>30.052889046111332</v>
       </c>
       <c r="I48">
         <v>107.625</v>
@@ -1919,28 +1919,28 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>353.73250958011113</v>
+        <v>288.4079820763734</v>
       </c>
       <c r="B49">
-        <v>312.67601597244163</v>
+        <v>257.16329612769948</v>
       </c>
       <c r="C49">
-        <v>172.89666838201762</v>
+        <v>180.46973156174263</v>
       </c>
       <c r="D49">
-        <v>149.99068630364116</v>
+        <v>126.8954178169042</v>
       </c>
       <c r="E49">
         <v>107.625</v>
       </c>
       <c r="F49">
-        <v>78.169003993110408</v>
+        <v>64.29082403192487</v>
       </c>
       <c r="G49">
         <v>107.625</v>
       </c>
       <c r="H49">
-        <v>37.497671575910289</v>
+        <v>31.72385445422605</v>
       </c>
       <c r="I49">
         <v>107.625</v>
@@ -1951,28 +1951,28 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>363.96328498203388</v>
+        <v>298.62017070098159</v>
       </c>
       <c r="B50">
-        <v>323.25516895387523</v>
+        <v>266.49825071222364</v>
       </c>
       <c r="C50">
-        <v>179.43697463376759</v>
+        <v>187.38068790715172</v>
       </c>
       <c r="D50">
-        <v>157.32683407895405</v>
+        <v>133.56677944936305</v>
       </c>
       <c r="E50">
         <v>107.625</v>
       </c>
       <c r="F50">
-        <v>80.813792238468807</v>
+        <v>66.624562678055909</v>
       </c>
       <c r="G50">
         <v>107.625</v>
       </c>
       <c r="H50">
-        <v>39.331708519738513</v>
+        <v>33.391694862340763</v>
       </c>
       <c r="I50">
         <v>107.625</v>
@@ -1983,28 +1983,28 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>373.55305588217175</v>
+        <v>308.6548642212569</v>
       </c>
       <c r="B51">
-        <v>333.53349570842977</v>
+        <v>275.75962575381959</v>
       </c>
       <c r="C51">
-        <v>185.96478088551754</v>
+        <v>194.2791442525608</v>
       </c>
       <c r="D51">
-        <v>164.65048185426693</v>
+        <v>140.22564108182192</v>
       </c>
       <c r="E51">
         <v>107.625</v>
       </c>
       <c r="F51">
-        <v>83.383373927107442</v>
+        <v>68.939906438454898</v>
       </c>
       <c r="G51">
         <v>107.625</v>
       </c>
       <c r="H51">
-        <v>41.162620463566732</v>
+        <v>35.05641027045548</v>
       </c>
       <c r="I51">
         <v>107.625</v>
@@ -2015,28 +2015,28 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>382.45504343943401</v>
+        <v>318.4926308316501</v>
       </c>
       <c r="B52">
-        <v>343.482650122172</v>
+        <v>284.93675076045031</v>
       </c>
       <c r="C52">
-        <v>192.4800871372675</v>
+        <v>201.16510059796988</v>
       </c>
       <c r="D52">
-        <v>171.96162962957982</v>
+        <v>146.8720027142808</v>
       </c>
       <c r="E52">
         <v>107.625</v>
       </c>
       <c r="F52">
-        <v>85.870662530543001</v>
+        <v>71.234187690112577</v>
       </c>
       <c r="G52">
         <v>107.625</v>
       </c>
       <c r="H52">
-        <v>42.990407407394954</v>
+        <v>36.718000678570199</v>
       </c>
       <c r="I52">
         <v>107.625</v>
@@ -2047,28 +2047,28 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>390.61198133707404</v>
+        <v>328.11402835229308</v>
       </c>
       <c r="B53">
-        <v>353.07430321719391</v>
+        <v>294.01895515273588</v>
       </c>
       <c r="C53">
-        <v>198.98289338901748</v>
+        <v>208.03855694337895</v>
       </c>
       <c r="D53">
-        <v>179.26027740489269</v>
+        <v>153.50586434673966</v>
       </c>
       <c r="E53">
         <v>107.625</v>
       </c>
       <c r="F53">
-        <v>88.268575804298479</v>
+        <v>73.504738788183971</v>
       </c>
       <c r="G53">
         <v>107.625</v>
       </c>
       <c r="H53">
-        <v>44.815069351223173</v>
+        <v>38.376466086684914</v>
       </c>
       <c r="I53">
         <v>107.625</v>
@@ -2079,28 +2079,28 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>397.97712406268425</v>
+        <v>337.4996284038416</v>
       </c>
       <c r="B54">
-        <v>362.28010937265799</v>
+        <v>302.99556674565105</v>
       </c>
       <c r="C54">
-        <v>205.47319964076743</v>
+        <v>214.89951328878803</v>
       </c>
       <c r="D54">
-        <v>186.54642518020557</v>
+        <v>160.12722597919853</v>
       </c>
       <c r="E54">
         <v>107.625</v>
       </c>
       <c r="F54">
-        <v>90.570027343164497</v>
+        <v>75.748891686412762</v>
       </c>
       <c r="G54">
         <v>107.625</v>
       </c>
       <c r="H54">
-        <v>46.636606295051394</v>
+        <v>40.031806494799632</v>
       </c>
       <c r="I54">
         <v>107.625</v>
@@ -2111,28 +2111,28 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>404.5072580313302</v>
+        <v>346.6299998309504</v>
       </c>
       <c r="B55">
-        <v>371.07167256058744</v>
+        <v>311.85591562594988</v>
       </c>
       <c r="C55">
-        <v>211.9510058925174</v>
+        <v>221.74796963419712</v>
       </c>
       <c r="D55">
-        <v>193.82007295551847</v>
+        <v>166.73608761165738</v>
       </c>
       <c r="E55">
         <v>107.625</v>
       </c>
       <c r="F55">
-        <v>92.767918140146861</v>
+        <v>77.963978906487469</v>
       </c>
       <c r="G55">
         <v>107.625</v>
       </c>
       <c r="H55">
-        <v>48.455018238879617</v>
+        <v>41.684021902914346</v>
       </c>
       <c r="I55">
         <v>107.625</v>
@@ -2143,28 +2143,28 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>411.2128580313302</v>
+        <v>355.48569847900376</v>
       </c>
       <c r="B56">
-        <v>377.77727256058745</v>
+        <v>320.58933053852712</v>
       </c>
       <c r="C56">
-        <v>218.41631214426735</v>
+        <v>228.58392597960619</v>
       </c>
       <c r="D56">
-        <v>201.08122073083135</v>
+        <v>173.33244924411625</v>
       </c>
       <c r="E56">
         <v>107.625</v>
       </c>
       <c r="F56">
-        <v>94.444318140146862</v>
+        <v>80.14733263463178</v>
       </c>
       <c r="G56">
         <v>107.625</v>
       </c>
       <c r="H56">
-        <v>50.270305182707837</v>
+        <v>43.333112311029062</v>
       </c>
       <c r="I56">
         <v>107.625</v>
@@ -2175,28 +2175,28 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>417.9184580313302</v>
+        <v>364.04732493389179</v>
       </c>
       <c r="B57">
-        <v>384.48287256058745</v>
+        <v>329.18514506597188</v>
       </c>
       <c r="C57">
-        <v>224.86911839601731</v>
+        <v>235.40738232501528</v>
       </c>
       <c r="D57">
-        <v>208.32986850614424</v>
+        <v>179.91631087657512</v>
       </c>
       <c r="E57">
         <v>107.625</v>
       </c>
       <c r="F57">
-        <v>96.120718140146863</v>
+        <v>82.29628626649297</v>
       </c>
       <c r="G57">
         <v>107.625</v>
       </c>
       <c r="H57">
-        <v>52.082467126536059</v>
+        <v>44.979077719143781</v>
       </c>
       <c r="I57">
         <v>107.625</v>
@@ -2207,28 +2207,28 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>424.62405803133021</v>
+        <v>372.29404082717116</v>
       </c>
       <c r="B58">
-        <v>391.18847256058746</v>
+        <v>337.63268113593324</v>
       </c>
       <c r="C58">
-        <v>231.30942464776729</v>
+        <v>242.21833867042434</v>
       </c>
       <c r="D58">
-        <v>215.56601628145711</v>
+        <v>186.48767250903398</v>
       </c>
       <c r="E58">
         <v>107.625</v>
       </c>
       <c r="F58">
-        <v>97.797118140146864</v>
+        <v>84.40817028398331</v>
       </c>
       <c r="G58">
         <v>107.625</v>
       </c>
       <c r="H58">
-        <v>53.891504070364277</v>
+        <v>46.621918127258496</v>
       </c>
       <c r="I58">
         <v>107.625</v>
@@ -2239,28 +2239,28 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>431.32965803133021</v>
+        <v>380.20904380677484</v>
       </c>
       <c r="B59">
-        <v>397.89407256058746</v>
+        <v>345.92126745246208</v>
       </c>
       <c r="C59">
-        <v>237.73723089951724</v>
+        <v>249.01679501583342</v>
       </c>
       <c r="D59">
-        <v>222.78966405676999</v>
+        <v>193.04653414149286</v>
       </c>
       <c r="E59">
         <v>107.625</v>
       </c>
       <c r="F59">
-        <v>99.473518140146865</v>
+        <v>86.480316863115519</v>
       </c>
       <c r="G59">
         <v>107.625</v>
       </c>
       <c r="H59">
-        <v>55.697416014192498</v>
+        <v>48.261633535373214</v>
       </c>
       <c r="I59">
         <v>107.625</v>
@@ -2271,28 +2271,28 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>438.03525803133022</v>
+        <v>387.77231111642197</v>
       </c>
       <c r="B60">
-        <v>404.59967256058746</v>
+        <v>354.04023684858879</v>
       </c>
       <c r="C60">
-        <v>244.15253715126721</v>
+        <v>255.80275136124251</v>
       </c>
       <c r="D60">
-        <v>230.00081183208289</v>
+        <v>199.59289577395171</v>
       </c>
       <c r="E60">
         <v>107.625</v>
       </c>
       <c r="F60">
-        <v>101.14991814014687</v>
+        <v>88.510059212147198</v>
       </c>
       <c r="G60">
         <v>107.625</v>
       </c>
       <c r="H60">
-        <v>57.500202958020722</v>
+        <v>49.898223943487928</v>
       </c>
       <c r="I60">
         <v>107.625</v>
@@ -2303,28 +2303,28 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>444.74085803133022</v>
+        <v>394.96399708988173</v>
       </c>
       <c r="B61">
-        <v>411.30527256058747</v>
+        <v>361.97898091417551</v>
       </c>
       <c r="C61">
-        <v>250.55534340301716</v>
+        <v>262.57620770665159</v>
       </c>
       <c r="D61">
-        <v>237.19945960739577</v>
+        <v>206.12675740641058</v>
       </c>
       <c r="E61">
         <v>107.625</v>
       </c>
       <c r="F61">
-        <v>102.82631814014687</v>
+        <v>90.494745228543877</v>
       </c>
       <c r="G61">
         <v>107.625</v>
       </c>
       <c r="H61">
-        <v>59.299864901848942</v>
+        <v>51.531689351602644</v>
       </c>
       <c r="I61">
         <v>107.625</v>
@@ -2335,28 +2335,28 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>451.44645803133022</v>
+        <v>401.76364072493135</v>
       </c>
       <c r="B62">
-        <v>418.01087256058747</v>
+        <v>369.72275317845106</v>
       </c>
       <c r="C62">
-        <v>256.94564965476707</v>
+        <v>269.33716405206064</v>
       </c>
       <c r="D62">
-        <v>244.38560738270866</v>
+        <v>212.64811903886945</v>
       </c>
       <c r="E62">
         <v>107.625</v>
       </c>
       <c r="F62">
-        <v>104.50271814014687</v>
+        <v>92.430688294612764</v>
       </c>
       <c r="G62">
         <v>107.625</v>
       </c>
       <c r="H62">
-        <v>61.096401845677164</v>
+        <v>53.162029759717363</v>
       </c>
       <c r="I62">
         <v>107.625</v>
@@ -2367,28 +2367,28 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>458.15205803133023</v>
+        <v>408.46924072493135</v>
       </c>
       <c r="B63">
-        <v>424.71647256058748</v>
+        <v>377.26828053790331</v>
       </c>
       <c r="C63">
-        <v>263.32345590651698</v>
+        <v>276.08562039746971</v>
       </c>
       <c r="D63">
-        <v>251.55925515802153</v>
+        <v>219.15698067132831</v>
       </c>
       <c r="E63">
         <v>107.625</v>
       </c>
       <c r="F63">
-        <v>106.17911814014687</v>
+        <v>94.317070134475827</v>
       </c>
       <c r="G63">
         <v>107.625</v>
       </c>
       <c r="H63">
-        <v>62.889813789505382</v>
+        <v>54.789245167832078</v>
       </c>
       <c r="I63">
         <v>107.625</v>
@@ -2399,28 +2399,28 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>464.85765803133023</v>
+        <v>415.17484072493136</v>
       </c>
       <c r="B64">
-        <v>431.42207256058748</v>
+        <v>383.97388053790331</v>
       </c>
       <c r="C64">
-        <v>269.68876215826691</v>
+        <v>282.82157674287879</v>
       </c>
       <c r="D64">
-        <v>258.72040293333436</v>
+        <v>225.65334230378718</v>
       </c>
       <c r="E64">
         <v>107.625</v>
       </c>
       <c r="F64">
-        <v>107.625</v>
+        <v>95.993470134475828</v>
       </c>
       <c r="G64">
         <v>107.625</v>
       </c>
       <c r="H64">
-        <v>64.680100733333589</v>
+        <v>56.413335575946796</v>
       </c>
       <c r="I64">
         <v>107.625</v>
@@ -2431,28 +2431,28 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>471.56325803133024</v>
+        <v>421.88044072493136</v>
       </c>
       <c r="B65">
-        <v>438.12767256058748</v>
+        <v>390.67948053790332</v>
       </c>
       <c r="C65">
-        <v>276.04156841001685</v>
+        <v>289.54503308828782</v>
       </c>
       <c r="D65">
-        <v>265.86905070864719</v>
+        <v>232.13720393624604</v>
       </c>
       <c r="E65">
         <v>107.625</v>
       </c>
       <c r="F65">
-        <v>107.625</v>
+        <v>97.669870134475829</v>
       </c>
       <c r="G65">
         <v>107.625</v>
       </c>
       <c r="H65">
-        <v>66.467262677161798</v>
+        <v>58.03430098406151</v>
       </c>
       <c r="I65">
         <v>107.625</v>
@@ -2463,28 +2463,28 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>478.26885803133024</v>
+        <v>428.58604072493137</v>
       </c>
       <c r="B66">
-        <v>444.83327256058749</v>
+        <v>397.38508053790332</v>
       </c>
       <c r="C66">
-        <v>282.3818746617668</v>
+        <v>296.25598943369687</v>
       </c>
       <c r="D66">
-        <v>273.00519848396004</v>
+        <v>238.6085655687049</v>
       </c>
       <c r="E66">
         <v>107.625</v>
       </c>
       <c r="F66">
-        <v>107.625</v>
+        <v>99.34627013447583</v>
       </c>
       <c r="G66">
         <v>107.625</v>
       </c>
       <c r="H66">
-        <v>68.251299620990011</v>
+        <v>59.652141392176226</v>
       </c>
       <c r="I66">
         <v>107.625</v>
@@ -2495,28 +2495,28 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>484.97445803133024</v>
+        <v>435.29164072493137</v>
       </c>
       <c r="B67">
-        <v>451.53887256058749</v>
+        <v>404.09068053790332</v>
       </c>
       <c r="C67">
-        <v>288.70968091351671</v>
+        <v>302.95444577910592</v>
       </c>
       <c r="D67">
-        <v>280.1288462592729</v>
+        <v>245.06742720116378</v>
       </c>
       <c r="E67">
         <v>107.625</v>
       </c>
       <c r="F67">
-        <v>107.625</v>
+        <v>101.02267013447583</v>
       </c>
       <c r="G67">
         <v>107.625</v>
       </c>
       <c r="H67">
-        <v>70.032211564818226</v>
+        <v>61.266856800290945</v>
       </c>
       <c r="I67">
         <v>107.625</v>
@@ -2527,28 +2527,28 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>491.68005803133025</v>
+        <v>441.99724072493137</v>
       </c>
       <c r="B68">
-        <v>458.2444725605875</v>
+        <v>410.79628053790333</v>
       </c>
       <c r="C68">
-        <v>295.02498716526662</v>
+        <v>309.64040212451499</v>
       </c>
       <c r="D68">
-        <v>287.23999403458578</v>
+        <v>251.51378883362264</v>
       </c>
       <c r="E68">
         <v>107.625</v>
       </c>
       <c r="F68">
-        <v>107.625</v>
+        <v>102.69907013447583</v>
       </c>
       <c r="G68">
         <v>107.625</v>
       </c>
       <c r="H68">
-        <v>71.809998508646444</v>
+        <v>62.87844720840566</v>
       </c>
       <c r="I68">
         <v>107.625</v>
@@ -2559,28 +2559,28 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>498.38565803133025</v>
+        <v>448.70284072493138</v>
       </c>
       <c r="B69">
-        <v>464.9500725605875</v>
+        <v>417.50188053790333</v>
       </c>
       <c r="C69">
-        <v>301.32779341701655</v>
+        <v>316.31385846992407</v>
       </c>
       <c r="D69">
-        <v>294.3386418098986</v>
+        <v>257.94765046608148</v>
       </c>
       <c r="E69">
         <v>107.625</v>
       </c>
       <c r="F69">
-        <v>107.625</v>
+        <v>104.37547013447583</v>
       </c>
       <c r="G69">
         <v>107.625</v>
       </c>
       <c r="H69">
-        <v>73.584660452474651</v>
+        <v>64.486912616520371</v>
       </c>
       <c r="I69">
         <v>107.625</v>
@@ -2591,28 +2591,28 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>505.09125803133026</v>
+        <v>455.40844072493138</v>
       </c>
       <c r="B70">
-        <v>471.6556725605875</v>
+        <v>424.20748053790334</v>
       </c>
       <c r="C70">
-        <v>307.61809966876649</v>
+        <v>322.9748148153331</v>
       </c>
       <c r="D70">
-        <v>301.42478958521144</v>
+        <v>264.36901209854034</v>
       </c>
       <c r="E70">
         <v>107.625</v>
       </c>
       <c r="F70">
-        <v>107.625</v>
+        <v>106.05187013447583</v>
       </c>
       <c r="G70">
         <v>107.625</v>
       </c>
       <c r="H70">
-        <v>75.356197396302861</v>
+        <v>66.092253024635085</v>
       </c>
       <c r="I70">
         <v>107.625</v>
@@ -2623,16 +2623,16 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>511.79685803133026</v>
+        <v>462.11404072493139</v>
       </c>
       <c r="B71">
-        <v>478.36127256058751</v>
+        <v>430.91308053790334</v>
       </c>
       <c r="C71">
-        <v>313.89590592051644</v>
+        <v>329.62327116074215</v>
       </c>
       <c r="D71">
-        <v>308.49843736052429</v>
+        <v>270.7778737309992</v>
       </c>
       <c r="E71">
         <v>107.625</v>
@@ -2644,7 +2644,7 @@
         <v>107.625</v>
       </c>
       <c r="H71">
-        <v>77.124609340131073</v>
+        <v>67.694468432749801</v>
       </c>
       <c r="I71">
         <v>107.625</v>
@@ -2655,16 +2655,16 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>518.50245803133021</v>
+        <v>468.81964072493139</v>
       </c>
       <c r="B72">
-        <v>485.06687256058751</v>
+        <v>437.61868053790334</v>
       </c>
       <c r="C72">
-        <v>320.16121217226635</v>
+        <v>336.25922750615121</v>
       </c>
       <c r="D72">
-        <v>315.55958513583715</v>
+        <v>277.17423536345802</v>
       </c>
       <c r="E72">
         <v>107.625</v>
@@ -2676,7 +2676,7 @@
         <v>107.625</v>
       </c>
       <c r="H72">
-        <v>78.889896283959288</v>
+        <v>69.293558840864506</v>
       </c>
       <c r="I72">
         <v>107.625</v>
@@ -2687,16 +2687,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>525.20805803133021</v>
+        <v>475.52524072493139</v>
       </c>
       <c r="B73">
-        <v>491.77247256058752</v>
+        <v>444.32428053790335</v>
       </c>
       <c r="C73">
-        <v>326.41401842401626</v>
+        <v>342.88268385156027</v>
       </c>
       <c r="D73">
-        <v>322.60823291115003</v>
+        <v>283.55809699591686</v>
       </c>
       <c r="E73">
         <v>107.625</v>
@@ -2708,7 +2708,7 @@
         <v>107.625</v>
       </c>
       <c r="H73">
-        <v>80.652058227787506</v>
+        <v>70.889524248979214</v>
       </c>
       <c r="I73">
         <v>107.625</v>
@@ -2719,16 +2719,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>531.91365803133021</v>
+        <v>482.2308407249314</v>
       </c>
       <c r="B74">
-        <v>498.47807256058752</v>
+        <v>451.02988053790335</v>
       </c>
       <c r="C74">
-        <v>332.65432467576619</v>
+        <v>349.49364019696935</v>
       </c>
       <c r="D74">
-        <v>329.64438068646285</v>
+        <v>289.9294586283757</v>
       </c>
       <c r="E74">
         <v>107.625</v>
@@ -2740,7 +2740,7 @@
         <v>107.625</v>
       </c>
       <c r="H74">
-        <v>82.411095171615713</v>
+        <v>72.482364657093925</v>
       </c>
       <c r="I74">
         <v>107.625</v>
@@ -2751,16 +2751,16 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>538.61925803133022</v>
+        <v>488.9364407249314</v>
       </c>
       <c r="B75">
-        <v>505.18367256058752</v>
+        <v>457.73548053790336</v>
       </c>
       <c r="C75">
-        <v>338.88213092751613</v>
+        <v>356.09209654237839</v>
       </c>
       <c r="D75">
-        <v>336.66802846177569</v>
+        <v>296.28832026083455</v>
       </c>
       <c r="E75">
         <v>107.625</v>
@@ -2772,7 +2772,7 @@
         <v>107.625</v>
       </c>
       <c r="H75">
-        <v>84.167007115443923</v>
+        <v>74.072080065208638</v>
       </c>
       <c r="I75">
         <v>107.625</v>
@@ -2783,16 +2783,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>545.32485803133022</v>
+        <v>495.64204072493141</v>
       </c>
       <c r="B76">
-        <v>511.88927256058753</v>
+        <v>464.44108053790336</v>
       </c>
       <c r="C76">
-        <v>345.09743717926608</v>
+        <v>362.67805288778743</v>
       </c>
       <c r="D76">
-        <v>343.67917623708854</v>
+        <v>302.63468189329342</v>
       </c>
       <c r="E76">
         <v>107.625</v>
@@ -2804,7 +2804,7 @@
         <v>107.625</v>
       </c>
       <c r="H76">
-        <v>85.919794059272135</v>
+        <v>75.658670473323355</v>
       </c>
       <c r="I76">
         <v>107.625</v>
@@ -2815,16 +2815,16 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>552.03045803133023</v>
+        <v>502.34764072493141</v>
       </c>
       <c r="B77">
-        <v>518.59487256058753</v>
+        <v>471.14668053790336</v>
       </c>
       <c r="C77">
-        <v>351.30024343101599</v>
+        <v>369.25150923319649</v>
       </c>
       <c r="D77">
-        <v>350.6778240124014</v>
+        <v>308.96854352575224</v>
       </c>
       <c r="E77">
         <v>107.625</v>
@@ -2836,7 +2836,7 @@
         <v>107.625</v>
       </c>
       <c r="H77">
-        <v>87.66945600310035</v>
+        <v>77.24213588143806</v>
       </c>
       <c r="I77">
         <v>107.625</v>
@@ -2847,16 +2847,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>558.73605803133023</v>
+        <v>509.05324072493141</v>
       </c>
       <c r="B78">
-        <v>525.30047256058754</v>
+        <v>477.85228053790337</v>
       </c>
       <c r="C78">
-        <v>357.4905496827659</v>
+        <v>375.81246557860555</v>
       </c>
       <c r="D78">
-        <v>357.66397178771427</v>
+        <v>315.28990515821107</v>
       </c>
       <c r="E78">
         <v>107.625</v>
@@ -2868,7 +2868,7 @@
         <v>107.625</v>
       </c>
       <c r="H78">
-        <v>89.415992946928569</v>
+        <v>78.822476289552768</v>
       </c>
       <c r="I78">
         <v>107.625</v>
@@ -2879,16 +2879,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>565.44165803133023</v>
+        <v>515.75884072493136</v>
       </c>
       <c r="B79">
-        <v>532.00607256058754</v>
+        <v>484.55788053790337</v>
       </c>
       <c r="C79">
-        <v>363.66835593451583</v>
+        <v>382.36092192401463</v>
       </c>
       <c r="D79">
-        <v>364.6376195630271</v>
+        <v>321.59876679066991</v>
       </c>
       <c r="E79">
         <v>107.625</v>
@@ -2900,7 +2900,7 @@
         <v>107.625</v>
       </c>
       <c r="H79">
-        <v>91.159404890756775</v>
+        <v>80.399691697667478</v>
       </c>
       <c r="I79">
         <v>107.625</v>
@@ -2911,16 +2911,16 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>572.14725803133024</v>
+        <v>522.46444072493136</v>
       </c>
       <c r="B80">
-        <v>538.71167256058754</v>
+        <v>491.26348053790338</v>
       </c>
       <c r="C80">
-        <v>369.83366218626577</v>
+        <v>388.89687826942367</v>
       </c>
       <c r="D80">
-        <v>371.59876733833994</v>
+        <v>327.89512842312877</v>
       </c>
       <c r="E80">
         <v>107.625</v>
@@ -2932,7 +2932,7 @@
         <v>107.625</v>
       </c>
       <c r="H80">
-        <v>92.899691834584985</v>
+        <v>81.973782105782192</v>
       </c>
       <c r="I80">
         <v>107.625</v>
@@ -2943,16 +2943,16 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>578.85285803133024</v>
+        <v>529.17004072493137</v>
       </c>
       <c r="B81">
-        <v>545.41727256058755</v>
+        <v>497.96908053790338</v>
       </c>
       <c r="C81">
-        <v>375.98646843801572</v>
+        <v>395.42033461483271</v>
       </c>
       <c r="D81">
-        <v>378.54741511365279</v>
+        <v>334.17899005558763</v>
       </c>
       <c r="E81">
         <v>107.625</v>
@@ -2964,7 +2964,7 @@
         <v>107.625</v>
       </c>
       <c r="H81">
-        <v>94.636853778413197</v>
+        <v>83.544747513896908</v>
       </c>
       <c r="I81">
         <v>107.625</v>
@@ -2975,16 +2975,16 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>585.55845803133025</v>
+        <v>535.87564072493137</v>
       </c>
       <c r="B82">
-        <v>552.12287256058755</v>
+        <v>504.67468053790338</v>
       </c>
       <c r="C82">
-        <v>382.12677468976563</v>
+        <v>401.93129096024177</v>
       </c>
       <c r="D82">
-        <v>385.48356288896565</v>
+        <v>340.45035168804645</v>
       </c>
       <c r="E82">
         <v>107.625</v>
@@ -2996,7 +2996,7 @@
         <v>107.625</v>
       </c>
       <c r="H82">
-        <v>96.370890722241413</v>
+        <v>85.112587922011613</v>
       </c>
       <c r="I82">
         <v>107.625</v>
@@ -3007,16 +3007,16 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>592.26405803133025</v>
+        <v>542.58124072493138</v>
       </c>
       <c r="B83">
-        <v>558.82847256058756</v>
+        <v>511.38028053790339</v>
       </c>
       <c r="C83">
-        <v>388.25458094151554</v>
+        <v>408.42974730565084</v>
       </c>
       <c r="D83">
-        <v>392.40721066427852</v>
+        <v>346.70921332050528</v>
       </c>
       <c r="E83">
         <v>107.625</v>
@@ -3028,7 +3028,7 @@
         <v>107.625</v>
       </c>
       <c r="H83">
-        <v>98.101802666069631</v>
+        <v>86.677303330126321</v>
       </c>
       <c r="I83">
         <v>107.625</v>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>598.96965803133025</v>
+        <v>549.28684072493138</v>
       </c>
       <c r="B84">
-        <v>565.53407256058756</v>
+        <v>518.08588053790334</v>
       </c>
       <c r="C84">
-        <v>394.36988719326547</v>
+        <v>414.91570365105991</v>
       </c>
       <c r="D84">
-        <v>399.31835843959135</v>
+        <v>352.95557495296413</v>
       </c>
       <c r="E84">
         <v>107.625</v>
@@ -3060,7 +3060,7 @@
         <v>107.625</v>
       </c>
       <c r="H84">
-        <v>99.829589609897837</v>
+        <v>88.238893738241032</v>
       </c>
       <c r="I84">
         <v>107.625</v>
@@ -3071,16 +3071,16 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>605.67525803133026</v>
+        <v>555.99244072493138</v>
       </c>
       <c r="B85">
-        <v>572.23967256058756</v>
+        <v>524.79148053790334</v>
       </c>
       <c r="C85">
-        <v>400.47269344501541</v>
+        <v>421.38915999646895</v>
       </c>
       <c r="D85">
-        <v>406.21700621490419</v>
+        <v>359.18943658542298</v>
       </c>
       <c r="E85">
         <v>107.625</v>
@@ -3092,7 +3092,7 @@
         <v>107.625</v>
       </c>
       <c r="H85">
-        <v>101.55425155372605</v>
+        <v>89.797359146355745</v>
       </c>
       <c r="I85">
         <v>107.625</v>
@@ -3103,16 +3103,16 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>612.38085803133026</v>
+        <v>562.69804072493139</v>
       </c>
       <c r="B86">
-        <v>578.94527256058757</v>
+        <v>531.49708053790334</v>
       </c>
       <c r="C86">
-        <v>406.56299969676536</v>
+        <v>427.85011634187799</v>
       </c>
       <c r="D86">
-        <v>413.10315399021704</v>
+        <v>365.41079821788185</v>
       </c>
       <c r="E86">
         <v>107.625</v>
@@ -3124,7 +3124,7 @@
         <v>107.625</v>
       </c>
       <c r="H86">
-        <v>103.27578849755426</v>
+        <v>91.352699554470462</v>
       </c>
       <c r="I86">
         <v>107.625</v>
@@ -3135,16 +3135,16 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>619.08645803133027</v>
+        <v>569.40364072493139</v>
       </c>
       <c r="B87">
-        <v>585.65087256058757</v>
+        <v>538.20268053790335</v>
       </c>
       <c r="C87">
-        <v>412.64080594851532</v>
+        <v>434.29857268728705</v>
       </c>
       <c r="D87">
-        <v>419.9768017655299</v>
+        <v>371.61965985034067</v>
       </c>
       <c r="E87">
         <v>107.625</v>
@@ -3156,7 +3156,7 @@
         <v>107.625</v>
       </c>
       <c r="H87">
-        <v>104.99420044138247</v>
+        <v>92.904914962585167</v>
       </c>
       <c r="I87">
         <v>107.625</v>
@@ -3167,16 +3167,16 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>625.79205803133027</v>
+        <v>576.1092407249314</v>
       </c>
       <c r="B88">
-        <v>592.35647256058758</v>
+        <v>544.90828053790335</v>
       </c>
       <c r="C88">
-        <v>418.70611220026524</v>
+        <v>440.74911428578957</v>
       </c>
       <c r="D88">
-        <v>426.83794954084277</v>
+        <v>377.8160214827995</v>
       </c>
       <c r="E88">
         <v>107.625</v>
@@ -3188,7 +3188,7 @@
         <v>107.625</v>
       </c>
       <c r="H88">
-        <v>106.70948738521069</v>
+        <v>94.454005370699875</v>
       </c>
       <c r="I88">
         <v>107.625</v>
@@ -3199,16 +3199,16 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>632.49765803133027</v>
+        <v>582.8148407249314</v>
       </c>
       <c r="B89">
-        <v>599.06207256058758</v>
+        <v>551.61388053790336</v>
       </c>
       <c r="C89">
-        <v>424.75891845201517</v>
+        <v>447.1996558842921</v>
       </c>
       <c r="D89">
-        <v>433.6865973161556</v>
+        <v>383.99988311525834</v>
       </c>
       <c r="E89">
         <v>107.625</v>
@@ -3220,7 +3220,7 @@
         <v>107.625</v>
       </c>
       <c r="H89">
-        <v>107.625</v>
+        <v>95.999970778814586</v>
       </c>
       <c r="I89">
         <v>107.625</v>
@@ -3231,16 +3231,16 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>639.20325803133028</v>
+        <v>589.5204407249314</v>
       </c>
       <c r="B90">
-        <v>605.76767256058758</v>
+        <v>558.31948053790336</v>
       </c>
       <c r="C90">
-        <v>430.79922470376511</v>
+        <v>453.65019748279462</v>
       </c>
       <c r="D90">
-        <v>440.53572662202436</v>
+        <v>390.1712447477172</v>
       </c>
       <c r="E90">
         <v>107.625</v>
@@ -3252,7 +3252,7 @@
         <v>107.625</v>
       </c>
       <c r="H90">
-        <v>107.625</v>
+        <v>97.542811186929299</v>
       </c>
       <c r="I90">
         <v>107.625</v>
@@ -3263,16 +3263,16 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>645.90885803133028</v>
+        <v>596.22604072493141</v>
       </c>
       <c r="B91">
-        <v>612.47327256058759</v>
+        <v>565.02508053790336</v>
       </c>
       <c r="C91">
-        <v>436.83493638233932</v>
+        <v>460.10073908129715</v>
       </c>
       <c r="D91">
-        <v>447.38485592789311</v>
+        <v>396.33010638017606</v>
       </c>
       <c r="E91">
         <v>107.625</v>
@@ -3284,7 +3284,7 @@
         <v>107.625</v>
       </c>
       <c r="H91">
-        <v>107.625</v>
+        <v>99.082526595044015</v>
       </c>
       <c r="I91">
         <v>107.625</v>
@@ -3295,16 +3295,16 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>652.61445803133029</v>
+        <v>602.93164072493141</v>
       </c>
       <c r="B92">
-        <v>619.17887256058759</v>
+        <v>571.73068053790337</v>
       </c>
       <c r="C92">
-        <v>442.87064806091354</v>
+        <v>466.55128067979967</v>
       </c>
       <c r="D92">
-        <v>454.23398523376187</v>
+        <v>402.47646801263488</v>
       </c>
       <c r="E92">
         <v>107.625</v>
@@ -3316,7 +3316,7 @@
         <v>107.625</v>
       </c>
       <c r="H92">
-        <v>107.625</v>
+        <v>100.61911700315872</v>
       </c>
       <c r="I92">
         <v>107.625</v>
@@ -3327,16 +3327,16 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>659.32005803133029</v>
+        <v>609.63724072493142</v>
       </c>
       <c r="B93">
-        <v>625.8844725605876</v>
+        <v>578.43628053790337</v>
       </c>
       <c r="C93">
-        <v>448.90635973948775</v>
+        <v>473.0018222783022</v>
       </c>
       <c r="D93">
-        <v>461.08311453963063</v>
+        <v>408.61032964509371</v>
       </c>
       <c r="E93">
         <v>107.625</v>
@@ -3348,7 +3348,7 @@
         <v>107.625</v>
       </c>
       <c r="H93">
-        <v>107.625</v>
+        <v>102.15258241127343</v>
       </c>
       <c r="I93">
         <v>107.625</v>
@@ -3359,16 +3359,16 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>666.02565803133029</v>
+        <v>616.34284072493142</v>
       </c>
       <c r="B94">
-        <v>632.5900725605876</v>
+        <v>585.14188053790338</v>
       </c>
       <c r="C94">
-        <v>454.94207141806197</v>
+        <v>479.45236387680472</v>
       </c>
       <c r="D94">
-        <v>467.93224384549939</v>
+        <v>414.73169127755256</v>
       </c>
       <c r="E94">
         <v>107.625</v>
@@ -3380,7 +3380,7 @@
         <v>107.625</v>
       </c>
       <c r="H94">
-        <v>107.625</v>
+        <v>103.68292281938814</v>
       </c>
       <c r="I94">
         <v>107.625</v>
@@ -3391,16 +3391,16 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>672.7312580313303</v>
+        <v>623.04844072493142</v>
       </c>
       <c r="B95">
-        <v>639.2956725605876</v>
+        <v>591.84748053790338</v>
       </c>
       <c r="C95">
-        <v>460.97778309663619</v>
+        <v>485.90290547530725</v>
       </c>
       <c r="D95">
-        <v>474.78137315136814</v>
+        <v>420.84055291001141</v>
       </c>
       <c r="E95">
         <v>107.625</v>
@@ -3412,7 +3412,7 @@
         <v>107.625</v>
       </c>
       <c r="H95">
-        <v>107.625</v>
+        <v>105.21013822750285</v>
       </c>
       <c r="I95">
         <v>107.625</v>
@@ -3423,16 +3423,16 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>679.4368580313303</v>
+        <v>629.75404072493143</v>
       </c>
       <c r="B96">
-        <v>646.00127256058761</v>
+        <v>598.55308053790338</v>
       </c>
       <c r="C96">
-        <v>467.0134947752104</v>
+        <v>492.35344707380978</v>
       </c>
       <c r="D96">
-        <v>481.6305024572369</v>
+        <v>426.93691454247028</v>
       </c>
       <c r="E96">
         <v>107.625</v>
@@ -3444,7 +3444,7 @@
         <v>107.625</v>
       </c>
       <c r="H96">
-        <v>107.625</v>
+        <v>106.73422863561757</v>
       </c>
       <c r="I96">
         <v>107.625</v>
@@ -3455,16 +3455,16 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>686.14245803133031</v>
+        <v>636.45964072493143</v>
       </c>
       <c r="B97">
-        <v>652.70687256058761</v>
+        <v>605.25868053790339</v>
       </c>
       <c r="C97">
-        <v>473.04920645378462</v>
+        <v>498.8039886723123</v>
       </c>
       <c r="D97">
-        <v>488.47963176310566</v>
+        <v>433.0207761749291</v>
       </c>
       <c r="E97">
         <v>107.625</v>
@@ -3487,16 +3487,16 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>692.84805803133031</v>
+        <v>643.16524072493144</v>
       </c>
       <c r="B98">
-        <v>659.41247256058762</v>
+        <v>611.96428053790339</v>
       </c>
       <c r="C98">
-        <v>479.08491813235884</v>
+        <v>505.25453027081483</v>
       </c>
       <c r="D98">
-        <v>495.32876106897442</v>
+        <v>439.10459755292601</v>
       </c>
       <c r="E98">
         <v>107.625</v>
@@ -3519,16 +3519,16 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>699.55365803133031</v>
+        <v>649.87084072493144</v>
       </c>
       <c r="B99">
-        <v>666.11807256058762</v>
+        <v>618.6698805379034</v>
       </c>
       <c r="C99">
-        <v>485.12062981093305</v>
+        <v>511.70507186931735</v>
       </c>
       <c r="D99">
-        <v>502.17789037484317</v>
+        <v>445.18841893092292</v>
       </c>
       <c r="E99">
         <v>107.625</v>
@@ -3551,16 +3551,16 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>706.25925803133032</v>
+        <v>656.57644072493144</v>
       </c>
       <c r="B100">
-        <v>672.82367256058762</v>
+        <v>625.3754805379034</v>
       </c>
       <c r="C100">
-        <v>491.15634148950727</v>
+        <v>518.15561346781988</v>
       </c>
       <c r="D100">
-        <v>509.02701968071193</v>
+        <v>451.27224030891983</v>
       </c>
       <c r="E100">
         <v>107.625</v>
@@ -3583,16 +3583,16 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>712.96485803133032</v>
+        <v>663.28204072493145</v>
       </c>
       <c r="B101">
-        <v>679.52927256058763</v>
+        <v>632.0810805379034</v>
       </c>
       <c r="C101">
-        <v>497.19205316808149</v>
+        <v>524.60615506632234</v>
       </c>
       <c r="D101">
-        <v>515.87614898658069</v>
+        <v>457.35606168691675</v>
       </c>
       <c r="E101">
         <v>107.625</v>
@@ -3615,16 +3615,16 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>719.67045803133033</v>
+        <v>669.98764072493145</v>
       </c>
       <c r="B102">
-        <v>686.23487256058763</v>
+        <v>638.78668053790341</v>
       </c>
       <c r="C102">
-        <v>503.2277648466557</v>
+        <v>531.05669666482481</v>
       </c>
       <c r="D102">
-        <v>522.7252782924495</v>
+        <v>463.43988306491366</v>
       </c>
       <c r="E102">
         <v>107.625</v>
@@ -3647,16 +3647,16 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>726.37605803133033</v>
+        <v>676.69324072493146</v>
       </c>
       <c r="B103">
-        <v>692.94047256058764</v>
+        <v>645.49228053790341</v>
       </c>
       <c r="C103">
-        <v>509.26347652522992</v>
+        <v>537.50723826332728</v>
       </c>
       <c r="D103">
-        <v>529.57440759831832</v>
+        <v>469.52370444291057</v>
       </c>
       <c r="E103">
         <v>107.625</v>
@@ -3679,16 +3679,16 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>733.08165803133033</v>
+        <v>683.39884072493146</v>
       </c>
       <c r="B104">
-        <v>699.64607256058764</v>
+        <v>652.19788053790342</v>
       </c>
       <c r="C104">
-        <v>515.29918820380408</v>
+        <v>543.95777986182975</v>
       </c>
       <c r="D104">
-        <v>536.42353690418713</v>
+        <v>475.60752582090748</v>
       </c>
       <c r="E104">
         <v>107.625</v>
@@ -3711,16 +3711,16 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>739.78725803133034</v>
+        <v>690.10444072493146</v>
       </c>
       <c r="B105">
-        <v>706.35167256058764</v>
+        <v>658.90348053790342</v>
       </c>
       <c r="C105">
-        <v>521.33489988237829</v>
+        <v>550.40832146033222</v>
       </c>
       <c r="D105">
-        <v>543.27266621005595</v>
+        <v>481.6913471989044</v>
       </c>
       <c r="E105">
         <v>107.625</v>
@@ -3743,16 +3743,16 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>746.49285803133034</v>
+        <v>696.81004072493147</v>
       </c>
       <c r="B106">
-        <v>713.05727256058765</v>
+        <v>665.60908053790342</v>
       </c>
       <c r="C106">
-        <v>527.37061156095251</v>
+        <v>556.85886305883469</v>
       </c>
       <c r="D106">
-        <v>550.12179551592476</v>
+        <v>487.77516857690131</v>
       </c>
       <c r="E106">
         <v>107.625</v>
@@ -3775,16 +3775,16 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>753.19845803133035</v>
+        <v>703.51564072493147</v>
       </c>
       <c r="B107">
-        <v>719.76287256058765</v>
+        <v>672.31468053790343</v>
       </c>
       <c r="C107">
-        <v>533.40632323952673</v>
+        <v>563.30940465733715</v>
       </c>
       <c r="D107">
-        <v>556.97092482179357</v>
+        <v>493.85898995489822</v>
       </c>
       <c r="E107">
         <v>107.625</v>
@@ -3807,16 +3807,16 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>759.90405803133035</v>
+        <v>710.22124072493148</v>
       </c>
       <c r="B108">
-        <v>726.46847256058766</v>
+        <v>679.02028053790343</v>
       </c>
       <c r="C108">
-        <v>539.44203491810094</v>
+        <v>569.75994625583962</v>
       </c>
       <c r="D108">
-        <v>563.82005412766239</v>
+        <v>499.94281133289513</v>
       </c>
       <c r="E108">
         <v>107.625</v>
@@ -3839,16 +3839,16 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>766.60965803133035</v>
+        <v>716.92684072493148</v>
       </c>
       <c r="B109">
-        <v>733.17407256058766</v>
+        <v>685.72588053790344</v>
       </c>
       <c r="C109">
-        <v>545.47774659667516</v>
+        <v>576.21048785434209</v>
       </c>
       <c r="D109">
-        <v>570.6691834335312</v>
+        <v>506.02663271089204</v>
       </c>
       <c r="E109">
         <v>107.625</v>
@@ -3871,16 +3871,16 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>773.31525803133036</v>
+        <v>723.63244072493148</v>
       </c>
       <c r="B110">
-        <v>739.87967256058766</v>
+        <v>692.43148053790344</v>
       </c>
       <c r="C110">
-        <v>551.51345827524938</v>
+        <v>582.66102945284456</v>
       </c>
       <c r="D110">
-        <v>577.51831273940002</v>
+        <v>512.11045408888901</v>
       </c>
       <c r="E110">
         <v>107.625</v>
@@ -3903,16 +3903,16 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>780.02085803133036</v>
+        <v>730.33804072493149</v>
       </c>
       <c r="B111">
-        <v>746.58527256058767</v>
+        <v>699.13708053790344</v>
       </c>
       <c r="C111">
-        <v>557.54916995382359</v>
+        <v>589.11157105134703</v>
       </c>
       <c r="D111">
-        <v>584.36744204526883</v>
+        <v>518.19427546688598</v>
       </c>
       <c r="E111">
         <v>107.625</v>
@@ -3935,16 +3935,16 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>786.72645803133037</v>
+        <v>737.04364072493149</v>
       </c>
       <c r="B112">
-        <v>753.29087256058767</v>
+        <v>705.84268053790345</v>
       </c>
       <c r="C112">
-        <v>563.58488163239781</v>
+        <v>595.5621126498495</v>
       </c>
       <c r="D112">
-        <v>591.21657135113765</v>
+        <v>524.27809684488295</v>
       </c>
       <c r="E112">
         <v>107.625</v>
@@ -3967,16 +3967,16 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>793.43205803133037</v>
+        <v>743.7492407249315</v>
       </c>
       <c r="B113">
-        <v>759.99647256058768</v>
+        <v>712.54828053790345</v>
       </c>
       <c r="C113">
-        <v>569.62059331097203</v>
+        <v>602.01265424835196</v>
       </c>
       <c r="D113">
-        <v>598.06570065700646</v>
+        <v>530.36191822287992</v>
       </c>
       <c r="E113">
         <v>107.625</v>
@@ -3999,16 +3999,16 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>800.13765803133037</v>
+        <v>750.4548407249315</v>
       </c>
       <c r="B114">
-        <v>766.70207256058768</v>
+        <v>719.25388053790346</v>
       </c>
       <c r="C114">
-        <v>575.65630498954624</v>
+        <v>608.46319584685443</v>
       </c>
       <c r="D114">
-        <v>604.91482996287527</v>
+        <v>536.44573960087689</v>
       </c>
       <c r="E114">
         <v>107.625</v>
@@ -4031,16 +4031,16 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>806.84325803133038</v>
+        <v>757.1604407249315</v>
       </c>
       <c r="B115">
-        <v>773.40767256058768</v>
+        <v>725.95948053790346</v>
       </c>
       <c r="C115">
-        <v>581.69201666812046</v>
+        <v>614.9137374453569</v>
       </c>
       <c r="D115">
-        <v>611.76395926874409</v>
+        <v>542.52956097887386</v>
       </c>
       <c r="E115">
         <v>107.625</v>
@@ -4063,16 +4063,16 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>813.54885803133038</v>
+        <v>763.86604072493151</v>
       </c>
       <c r="B116">
-        <v>780.11327256058769</v>
+        <v>732.66508053790346</v>
       </c>
       <c r="C116">
-        <v>587.72772834669468</v>
+        <v>621.36427904385937</v>
       </c>
       <c r="D116">
-        <v>618.6130885746129</v>
+        <v>548.61338235687083</v>
       </c>
       <c r="E116">
         <v>107.625</v>
@@ -4095,16 +4095,16 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>820.25445803133039</v>
+        <v>770.57164072493151</v>
       </c>
       <c r="B117">
-        <v>786.81887256058769</v>
+        <v>739.37068053790347</v>
       </c>
       <c r="C117">
-        <v>593.76344002526889</v>
+        <v>627.81482064236184</v>
       </c>
       <c r="D117">
-        <v>625.46221788048172</v>
+        <v>554.6972037348678</v>
       </c>
       <c r="E117">
         <v>107.625</v>
@@ -4127,16 +4127,16 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>826.96005803133039</v>
+        <v>777.27724072493152</v>
       </c>
       <c r="B118">
-        <v>793.5244725605877</v>
+        <v>746.07628053790347</v>
       </c>
       <c r="C118">
-        <v>599.79915170384311</v>
+        <v>634.26536224086431</v>
       </c>
       <c r="D118">
-        <v>632.31134718635053</v>
+        <v>560.78102511286477</v>
       </c>
       <c r="E118">
         <v>107.625</v>
@@ -4159,16 +4159,16 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>833.66565803133039</v>
+        <v>783.98284072493152</v>
       </c>
       <c r="B119">
-        <v>800.2300725605877</v>
+        <v>752.78188053790348</v>
       </c>
       <c r="C119">
-        <v>605.83486338241732</v>
+        <v>640.71590383936677</v>
       </c>
       <c r="D119">
-        <v>639.16047649221935</v>
+        <v>566.86484649086174</v>
       </c>
       <c r="E119">
         <v>107.625</v>
@@ -4191,16 +4191,16 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>840.3712580313304</v>
+        <v>790.68844072493152</v>
       </c>
       <c r="B120">
-        <v>806.9356725605877</v>
+        <v>759.48748053790348</v>
       </c>
       <c r="C120">
-        <v>611.87057506099154</v>
+        <v>647.16644543786924</v>
       </c>
       <c r="D120">
-        <v>646.00960579808816</v>
+        <v>572.94866786885871</v>
       </c>
       <c r="E120">
         <v>107.625</v>
@@ -4223,16 +4223,16 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>847.0768580313304</v>
+        <v>797.39404072493153</v>
       </c>
       <c r="B121">
-        <v>813.64127256058771</v>
+        <v>766.19308053790348</v>
       </c>
       <c r="C121">
-        <v>617.90628673956576</v>
+        <v>653.61698703637171</v>
       </c>
       <c r="D121">
-        <v>652.85873510395697</v>
+        <v>579.03248924685568</v>
       </c>
       <c r="E121">
         <v>107.625</v>
@@ -4255,16 +4255,16 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>853.78245803133041</v>
+        <v>804.09964072493153</v>
       </c>
       <c r="B122">
-        <v>820.34687256058771</v>
+        <v>772.89868053790349</v>
       </c>
       <c r="C122">
-        <v>623.94199841813997</v>
+        <v>660.06752863487418</v>
       </c>
       <c r="D122">
-        <v>659.70786440982579</v>
+        <v>585.11631062485264</v>
       </c>
       <c r="E122">
         <v>107.625</v>
@@ -4287,16 +4287,16 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>860.48805803133041</v>
+        <v>810.80524072493154</v>
       </c>
       <c r="B123">
-        <v>827.05247256058772</v>
+        <v>779.60428053790349</v>
       </c>
       <c r="C123">
-        <v>629.97771009671419</v>
+        <v>666.51807023337665</v>
       </c>
       <c r="D123">
-        <v>666.5569937156946</v>
+        <v>591.20013200284961</v>
       </c>
       <c r="E123">
         <v>107.625</v>
@@ -4319,16 +4319,16 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>867.19365803133041</v>
+        <v>817.51084072493154</v>
       </c>
       <c r="B124">
-        <v>833.75807256058772</v>
+        <v>786.3098805379035</v>
       </c>
       <c r="C124">
-        <v>636.01342177528841</v>
+        <v>672.96861183187912</v>
       </c>
       <c r="D124">
-        <v>673.40612302156342</v>
+        <v>597.28395338084658</v>
       </c>
       <c r="E124">
         <v>107.625</v>
@@ -4351,16 +4351,16 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>873.89925803133042</v>
+        <v>824.21644072493154</v>
       </c>
       <c r="B125">
-        <v>840.46367256058772</v>
+        <v>793.0154805379035</v>
       </c>
       <c r="C125">
-        <v>642.04913345386262</v>
+        <v>679.41915343038158</v>
       </c>
       <c r="D125">
-        <v>680.25525232743223</v>
+        <v>603.36777475884355</v>
       </c>
       <c r="E125">
         <v>107.625</v>
@@ -4383,16 +4383,16 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>880.60485803133042</v>
+        <v>830.92204072493155</v>
       </c>
       <c r="B126">
-        <v>847.16927256058773</v>
+        <v>799.7210805379035</v>
       </c>
       <c r="C126">
-        <v>648.08484513243684</v>
+        <v>685.86969502888405</v>
       </c>
       <c r="D126">
-        <v>687.10438163330105</v>
+        <v>609.45159613684052</v>
       </c>
       <c r="E126">
         <v>107.625</v>
@@ -4415,16 +4415,16 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>887.31045803133043</v>
+        <v>837.62764072493155</v>
       </c>
       <c r="B127">
-        <v>853.87487256058773</v>
+        <v>806.42668053790351</v>
       </c>
       <c r="C127">
-        <v>654.12055681101106</v>
+        <v>692.32023662738652</v>
       </c>
       <c r="D127">
-        <v>693.95351093916986</v>
+        <v>615.53541751483749</v>
       </c>
       <c r="E127">
         <v>107.625</v>
@@ -4447,16 +4447,16 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>894.01605803133043</v>
+        <v>844.33324072493156</v>
       </c>
       <c r="B128">
-        <v>860.58047256058774</v>
+        <v>813.13228053790351</v>
       </c>
       <c r="C128">
-        <v>660.15626848958527</v>
+        <v>698.77077822588899</v>
       </c>
       <c r="D128">
-        <v>700.80264024503867</v>
+        <v>621.61923889283446</v>
       </c>
       <c r="E128">
         <v>107.625</v>
@@ -4479,16 +4479,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>900.72165803133043</v>
+        <v>851.03884072493156</v>
       </c>
       <c r="B129">
-        <v>867.28607256058774</v>
+        <v>819.83788053790352</v>
       </c>
       <c r="C129">
-        <v>666.19198016815949</v>
+        <v>705.22131982439146</v>
       </c>
       <c r="D129">
-        <v>707.65176955090749</v>
+        <v>627.70306027083143</v>
       </c>
       <c r="E129">
         <v>107.625</v>
@@ -4511,16 +4511,16 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>907.42725803133044</v>
+        <v>857.74444072493156</v>
       </c>
       <c r="B130">
-        <v>873.99167256058774</v>
+        <v>826.54348053790352</v>
       </c>
       <c r="C130">
-        <v>672.22769184673371</v>
+        <v>711.67186142289393</v>
       </c>
       <c r="D130">
-        <v>714.5008988567763</v>
+        <v>633.7868816488284</v>
       </c>
       <c r="E130">
         <v>107.625</v>
@@ -4543,16 +4543,16 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>914.13285803133044</v>
+        <v>864.45004072493157</v>
       </c>
       <c r="B131">
-        <v>880.69727256058775</v>
+        <v>833.24908053790352</v>
       </c>
       <c r="C131">
-        <v>678.26340352530792</v>
+        <v>718.12240302139639</v>
       </c>
       <c r="D131">
-        <v>721.35002816264512</v>
+        <v>639.87070302682537</v>
       </c>
       <c r="E131">
         <v>107.625</v>
@@ -4575,16 +4575,16 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>920.83845803133045</v>
+        <v>871.15564072493157</v>
       </c>
       <c r="B132">
-        <v>887.40287256058775</v>
+        <v>839.95468053790353</v>
       </c>
       <c r="C132">
-        <v>684.29911520388214</v>
+        <v>724.57294461989886</v>
       </c>
       <c r="D132">
-        <v>728.19915746851393</v>
+        <v>645.95452440482234</v>
       </c>
       <c r="E132">
         <v>107.625</v>
@@ -4607,16 +4607,16 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>927.54405803133045</v>
+        <v>877.86124072493158</v>
       </c>
       <c r="B133">
-        <v>894.10847256058776</v>
+        <v>846.66028053790353</v>
       </c>
       <c r="C133">
-        <v>690.33482688245635</v>
+        <v>731.02348621840133</v>
       </c>
       <c r="D133">
-        <v>735.04828677438275</v>
+        <v>652.03834578281931</v>
       </c>
       <c r="E133">
         <v>107.625</v>
@@ -4639,16 +4639,16 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>934.24965803133045</v>
+        <v>884.56684072493158</v>
       </c>
       <c r="B134">
-        <v>900.81407256058776</v>
+        <v>853.36588053790354</v>
       </c>
       <c r="C134">
-        <v>696.37053856103057</v>
+        <v>737.4740278169038</v>
       </c>
       <c r="D134">
-        <v>741.89741608025156</v>
+        <v>658.12216716081628</v>
       </c>
       <c r="E134">
         <v>107.625</v>
@@ -4671,16 +4671,16 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>940.95525803133046</v>
+        <v>891.27244072493158</v>
       </c>
       <c r="B135">
-        <v>907.51967256058776</v>
+        <v>860.07148053790354</v>
       </c>
       <c r="C135">
-        <v>702.40625023960479</v>
+        <v>743.92456941540627</v>
       </c>
       <c r="D135">
-        <v>748.74654538612037</v>
+        <v>664.20598853881324</v>
       </c>
       <c r="E135">
         <v>107.625</v>
@@ -4703,16 +4703,16 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>947.66085803133046</v>
+        <v>897.97804072493159</v>
       </c>
       <c r="B136">
-        <v>914.22527256058777</v>
+        <v>866.77708053790354</v>
       </c>
       <c r="C136">
-        <v>708.441961918179</v>
+        <v>750.37511101390874</v>
       </c>
       <c r="D136">
-        <v>755.59567469198919</v>
+        <v>670.28980991681021</v>
       </c>
       <c r="E136">
         <v>107.625</v>
@@ -4735,16 +4735,16 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>954.36645803133047</v>
+        <v>904.68364072493159</v>
       </c>
       <c r="B137">
-        <v>920.93087256058777</v>
+        <v>873.48268053790355</v>
       </c>
       <c r="C137">
-        <v>714.47767359675322</v>
+        <v>756.8256526124112</v>
       </c>
       <c r="D137">
-        <v>762.444803997858</v>
+        <v>676.37363129480718</v>
       </c>
       <c r="E137">
         <v>107.625</v>
@@ -4767,16 +4767,16 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>961.07205803133047</v>
+        <v>911.3892407249316</v>
       </c>
       <c r="B138">
-        <v>927.63647256058778</v>
+        <v>880.18828053790355</v>
       </c>
       <c r="C138">
-        <v>720.51338527532744</v>
+        <v>763.27619421091367</v>
       </c>
       <c r="D138">
-        <v>769.29393330372682</v>
+        <v>682.45745267280415</v>
       </c>
       <c r="E138">
         <v>107.625</v>
@@ -4799,16 +4799,16 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>967.77765803133047</v>
+        <v>918.0948407249316</v>
       </c>
       <c r="B139">
-        <v>934.34207256058778</v>
+        <v>886.89388053790356</v>
       </c>
       <c r="C139">
-        <v>726.54909695390165</v>
+        <v>769.72673580941614</v>
       </c>
       <c r="D139">
-        <v>776.14306260959563</v>
+        <v>688.54127405080112</v>
       </c>
       <c r="E139">
         <v>107.625</v>
@@ -4831,16 +4831,16 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>974.48325803133048</v>
+        <v>924.8004407249316</v>
       </c>
       <c r="B140">
-        <v>941.04767256058778</v>
+        <v>893.59948053790356</v>
       </c>
       <c r="C140">
-        <v>732.58480863247587</v>
+        <v>776.17727740791861</v>
       </c>
       <c r="D140">
-        <v>782.99219191546445</v>
+        <v>694.62509542879809</v>
       </c>
       <c r="E140">
         <v>107.625</v>
@@ -4863,16 +4863,16 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>981.18885803133048</v>
+        <v>931.50604072493161</v>
       </c>
       <c r="B141">
-        <v>947.75327256058779</v>
+        <v>900.30508053790356</v>
       </c>
       <c r="C141">
-        <v>738.62052031105009</v>
+        <v>782.62781900642108</v>
       </c>
       <c r="D141">
-        <v>789.84132122133326</v>
+        <v>700.70891680679506</v>
       </c>
       <c r="E141">
         <v>107.625</v>
@@ -4895,16 +4895,16 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>987.89445803133049</v>
+        <v>938.21164072493161</v>
       </c>
       <c r="B142">
-        <v>954.45887256058779</v>
+        <v>907.01068053790357</v>
       </c>
       <c r="C142">
-        <v>744.6562319896243</v>
+        <v>789.07836060492355</v>
       </c>
       <c r="D142">
-        <v>796.69045052720207</v>
+        <v>706.79273818479203</v>
       </c>
       <c r="E142">
         <v>107.625</v>
@@ -4927,16 +4927,16 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>994.60005803133049</v>
+        <v>944.91724072493162</v>
       </c>
       <c r="B143">
-        <v>961.1644725605878</v>
+        <v>913.71628053790357</v>
       </c>
       <c r="C143">
-        <v>750.69194366819852</v>
+        <v>795.52890220342601</v>
       </c>
       <c r="D143">
-        <v>803.53957983307089</v>
+        <v>712.876559562789</v>
       </c>
       <c r="E143">
         <v>107.625</v>
@@ -4959,16 +4959,16 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>1001.3056580313305</v>
+        <v>951.62284072493162</v>
       </c>
       <c r="B144">
-        <v>967.8700725605878</v>
+        <v>920.42188053790358</v>
       </c>
       <c r="C144">
-        <v>756.72765534677274</v>
+        <v>801.97944380192848</v>
       </c>
       <c r="D144">
-        <v>810.3887091389397</v>
+        <v>718.96038094078597</v>
       </c>
       <c r="E144">
         <v>107.625</v>
@@ -4991,16 +4991,16 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>1008.0112580313305</v>
+        <v>958.32844072493162</v>
       </c>
       <c r="B145">
-        <v>974.5756725605878</v>
+        <v>927.12748053790358</v>
       </c>
       <c r="C145">
-        <v>762.76336702534695</v>
+        <v>808.42998540043095</v>
       </c>
       <c r="D145">
-        <v>817.23783844480852</v>
+        <v>725.04420231878294</v>
       </c>
       <c r="E145">
         <v>107.625</v>
@@ -5023,16 +5023,16 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>1014.7168580313305</v>
+        <v>965.03404072493163</v>
       </c>
       <c r="B146">
-        <v>981.28127256058781</v>
+        <v>933.83308053790358</v>
       </c>
       <c r="C146">
-        <v>768.79907870392117</v>
+        <v>814.88052699893342</v>
       </c>
       <c r="D146">
-        <v>824.08696775067733</v>
+        <v>731.12802369677991</v>
       </c>
       <c r="E146">
         <v>107.625</v>
@@ -5055,16 +5055,16 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>1021.4224580313305</v>
+        <v>971.73964072493163</v>
       </c>
       <c r="B147">
-        <v>987.98687256058781</v>
+        <v>940.53868053790359</v>
       </c>
       <c r="C147">
-        <v>774.83479038249538</v>
+        <v>821.33106859743589</v>
       </c>
       <c r="D147">
-        <v>830.93609705654615</v>
+        <v>737.21184507477687</v>
       </c>
       <c r="E147">
         <v>107.625</v>
@@ -5087,16 +5087,16 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>1028.1280580313305</v>
+        <v>978.44524072493164</v>
       </c>
       <c r="B148">
-        <v>994.69247256058782</v>
+        <v>947.24428053790359</v>
       </c>
       <c r="C148">
-        <v>780.8705020610696</v>
+        <v>827.78161019593836</v>
       </c>
       <c r="D148">
-        <v>837.78522636241496</v>
+        <v>743.29566645277384</v>
       </c>
       <c r="E148">
         <v>107.625</v>
@@ -5119,16 +5119,16 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>1034.8336580313305</v>
+        <v>985.15084072493164</v>
       </c>
       <c r="B149">
-        <v>1001.3980725605878</v>
+        <v>953.9498805379036</v>
       </c>
       <c r="C149">
-        <v>786.90621373964382</v>
+        <v>834.23215179444082</v>
       </c>
       <c r="D149">
-        <v>844.63435566828377</v>
+        <v>749.37948783077081</v>
       </c>
       <c r="E149">
         <v>107.625</v>
@@ -5151,16 +5151,16 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>1041.5392580313305</v>
+        <v>991.85644072493164</v>
       </c>
       <c r="B150">
-        <v>1008.1036725605878</v>
+        <v>960.6554805379036</v>
       </c>
       <c r="C150">
-        <v>792.94192541821803</v>
+        <v>840.68269339294329</v>
       </c>
       <c r="D150">
-        <v>851.48348497415259</v>
+        <v>755.46330920876778</v>
       </c>
       <c r="E150">
         <v>107.625</v>
@@ -5183,16 +5183,16 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>1048.2448580313305</v>
+        <v>998.56204072493165</v>
       </c>
       <c r="B151">
-        <v>1014.8092725605878</v>
+        <v>967.3610805379036</v>
       </c>
       <c r="C151">
-        <v>798.97763709679225</v>
+        <v>847.13323499144576</v>
       </c>
       <c r="D151">
-        <v>858.3326142800214</v>
+        <v>761.54713058676475</v>
       </c>
       <c r="E151">
         <v>107.625</v>
@@ -5215,16 +5215,16 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>1054.9504580313305</v>
+        <v>1005.2676407249317</v>
       </c>
       <c r="B152">
-        <v>1021.5148725605878</v>
+        <v>974.06668053790361</v>
       </c>
       <c r="C152">
-        <v>805.01334877536647</v>
+        <v>853.58377658994823</v>
       </c>
       <c r="D152">
-        <v>865.18174358589022</v>
+        <v>767.63095196476172</v>
       </c>
       <c r="E152">
         <v>107.625</v>
@@ -5247,16 +5247,16 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>1061.6560580313305</v>
+        <v>1011.9732407249317</v>
       </c>
       <c r="B153">
-        <v>1028.2204725605877</v>
+        <v>980.77228053790361</v>
       </c>
       <c r="C153">
-        <v>811.04906045394068</v>
+        <v>860.0343181884507</v>
       </c>
       <c r="D153">
-        <v>872.03087289175903</v>
+        <v>773.71477334275869</v>
       </c>
       <c r="E153">
         <v>107.625</v>
@@ -5279,16 +5279,16 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>1068.3616580313305</v>
+        <v>1018.6788407249317</v>
       </c>
       <c r="B154">
-        <v>1034.9260725605877</v>
+        <v>987.47788053790362</v>
       </c>
       <c r="C154">
-        <v>817.0847721325149</v>
+        <v>866.48485978695317</v>
       </c>
       <c r="D154">
-        <v>878.88000219762785</v>
+        <v>779.79859472075566</v>
       </c>
       <c r="E154">
         <v>107.625</v>
@@ -5311,16 +5311,16 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>1075.0672580313305</v>
+        <v>1025.3844407249317</v>
       </c>
       <c r="B155">
-        <v>1041.6316725605877</v>
+        <v>994.18348053790362</v>
       </c>
       <c r="C155">
-        <v>823.12048381108912</v>
+        <v>872.93540138545563</v>
       </c>
       <c r="D155">
-        <v>885.72913150349666</v>
+        <v>785.88241609875263</v>
       </c>
       <c r="E155">
         <v>107.625</v>
@@ -5343,16 +5343,16 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>1081.7728580313305</v>
+        <v>1032.0900407249317</v>
       </c>
       <c r="B156">
-        <v>1048.3372725605877</v>
+        <v>1000.8890805379036</v>
       </c>
       <c r="C156">
-        <v>829.15619548966333</v>
+        <v>879.3859429839581</v>
       </c>
       <c r="D156">
-        <v>892.57826080936547</v>
+        <v>791.9662374767496</v>
       </c>
       <c r="E156">
         <v>107.625</v>
@@ -5375,16 +5375,16 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>1088.4784580313305</v>
+        <v>1038.7956407249317</v>
       </c>
       <c r="B157">
-        <v>1055.0428725605877</v>
+        <v>1007.5946805379036</v>
       </c>
       <c r="C157">
-        <v>835.19190716823755</v>
+        <v>885.83648458246057</v>
       </c>
       <c r="D157">
-        <v>899.42739011523429</v>
+        <v>798.05005885474657</v>
       </c>
       <c r="E157">
         <v>107.625</v>
@@ -5407,16 +5407,16 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>1095.1840580313306</v>
+        <v>1045.5012407249317</v>
       </c>
       <c r="B158">
-        <v>1061.7484725605877</v>
+        <v>1014.3002805379036</v>
       </c>
       <c r="C158">
-        <v>841.22761884681177</v>
+        <v>892.28702618096304</v>
       </c>
       <c r="D158">
-        <v>906.2765194211031</v>
+        <v>804.13388023274354</v>
       </c>
       <c r="E158">
         <v>107.625</v>
@@ -5439,16 +5439,16 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>1101.8896580313306</v>
+        <v>1052.2068407249317</v>
       </c>
       <c r="B159">
-        <v>1068.4540725605877</v>
+        <v>1021.0058805379036</v>
       </c>
       <c r="C159">
-        <v>847.26333052538598</v>
+        <v>898.73756777946551</v>
       </c>
       <c r="D159">
-        <v>913.12564872697192</v>
+        <v>810.21770161074051</v>
       </c>
       <c r="E159">
         <v>107.625</v>
@@ -5471,16 +5471,16 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>1108.5952580313306</v>
+        <v>1058.9124407249317</v>
       </c>
       <c r="B160">
-        <v>1075.1596725605878</v>
+        <v>1027.7114805379035</v>
       </c>
       <c r="C160">
-        <v>853.2990422039602</v>
+        <v>905.18810937796798</v>
       </c>
       <c r="D160">
-        <v>919.97477803284073</v>
+        <v>816.30152298873747</v>
       </c>
       <c r="E160">
         <v>107.625</v>

</xml_diff>